<commit_message>
add new function for subject analysis
</commit_message>
<xml_diff>
--- a/NewOldTask-analysis/variantLIST.xlsx
+++ b/NewOldTask-analysis/variantLIST.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="841">
   <si>
     <t>Right</t>
   </si>
@@ -354,6 +354,1581 @@
   </si>
   <si>
     <t>Right</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>AMC_PY21NO05</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO09</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO12</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO13</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO16</t>
+  </si>
+  <si>
+    <t>EDF</t>
+  </si>
+  <si>
+    <t>NO5171621.edf</t>
+  </si>
+  <si>
+    <t>NO5271621.edf</t>
+  </si>
+  <si>
+    <t>NO5171821.edf</t>
+  </si>
+  <si>
+    <t>NO5271821.edf</t>
+  </si>
+  <si>
+    <t>NO20221615110.edf</t>
+  </si>
+  <si>
+    <t>NO202216152152.edf</t>
+  </si>
+  <si>
+    <t>NO202217121946.edf</t>
+  </si>
+  <si>
+    <t>NO202217122836.edf</t>
+  </si>
+  <si>
+    <t>NO20221811515.edf</t>
+  </si>
+  <si>
+    <t>NO20221812052.edf</t>
+  </si>
+  <si>
+    <t>NO52022420124541.edf</t>
+  </si>
+  <si>
+    <t>NO52022420125453.edf</t>
+  </si>
+  <si>
+    <t>NO202252915450.edf</t>
+  </si>
+  <si>
+    <t>NO2022529151348.edf</t>
+  </si>
+  <si>
+    <t>NO202261115116.edf</t>
+  </si>
+  <si>
+    <t>NO20226111597.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105026.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105927.edf</t>
+  </si>
+  <si>
+    <t>NO2022826164318.edf</t>
+  </si>
+  <si>
+    <t>NO202282616539.edf</t>
+  </si>
+  <si>
+    <t>NO20228261764.edf</t>
+  </si>
+  <si>
+    <t>NO2022826171650.edf</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>Behavior</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221615110.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202216152152.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217121946.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217122836.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221811515.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221812052.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420124541.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420125453.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202252915450.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022529151348.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202261115116.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520226111597.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105026.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105927.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826164318.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202282616539.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520228261764.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826171650.txt</t>
+  </si>
+  <si>
+    <t>MatFile</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Learn_5171621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Recog_5271621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Learn_5171821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Recog_5271821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Learn_20221615110.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Recog_202216152152.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Learn_202217121946.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Recog_202217122836.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Learn_20221811515.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Recog_20221812052.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Learn_52022420124541.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Recog_52022420125453.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Learn_202252915450.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Recog_2022529151348.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Learn_202261115116.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Recog_20226111597.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Learn_2022527105026.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Recog_2022527105927.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Learn_2022826164318.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Recog_202282616539.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Learn_20228261764.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Recog_2022826171650.mat</t>
+  </si>
+  <si>
+    <t>Eye2Use</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>AMC_PY21NO05</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO09</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO12</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO13</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO16</t>
+  </si>
+  <si>
+    <t>EDF</t>
+  </si>
+  <si>
+    <t>NO5171621.edf</t>
+  </si>
+  <si>
+    <t>NO5271621.edf</t>
+  </si>
+  <si>
+    <t>NO5171821.edf</t>
+  </si>
+  <si>
+    <t>NO5271821.edf</t>
+  </si>
+  <si>
+    <t>NO20221615110.edf</t>
+  </si>
+  <si>
+    <t>NO202216152152.edf</t>
+  </si>
+  <si>
+    <t>NO202217121946.edf</t>
+  </si>
+  <si>
+    <t>NO202217122836.edf</t>
+  </si>
+  <si>
+    <t>NO20221811515.edf</t>
+  </si>
+  <si>
+    <t>NO20221812052.edf</t>
+  </si>
+  <si>
+    <t>NO52022420124541.edf</t>
+  </si>
+  <si>
+    <t>NO52022420125453.edf</t>
+  </si>
+  <si>
+    <t>NO202252915450.edf</t>
+  </si>
+  <si>
+    <t>NO2022529151348.edf</t>
+  </si>
+  <si>
+    <t>NO202261115116.edf</t>
+  </si>
+  <si>
+    <t>NO20226111597.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105026.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105927.edf</t>
+  </si>
+  <si>
+    <t>NO2022826164318.edf</t>
+  </si>
+  <si>
+    <t>NO202282616539.edf</t>
+  </si>
+  <si>
+    <t>NO20228261764.edf</t>
+  </si>
+  <si>
+    <t>NO2022826171650.edf</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>Behavior</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221615110.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202216152152.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217121946.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217122836.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221811515.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221812052.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420124541.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420125453.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202252915450.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022529151348.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202261115116.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520226111597.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105026.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105927.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826164318.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202282616539.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520228261764.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826171650.txt</t>
+  </si>
+  <si>
+    <t>MatFile</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Learn_5171621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Recog_5271621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Learn_5171821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Recog_5271821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Learn_20221615110.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Recog_202216152152.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Learn_202217121946.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Recog_202217122836.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Learn_20221811515.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Recog_20221812052.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Learn_52022420124541.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Recog_52022420125453.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Learn_202252915450.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Recog_2022529151348.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Learn_202261115116.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Recog_20226111597.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Learn_2022527105026.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Recog_2022527105927.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Learn_2022826164318.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Recog_202282616539.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Learn_20228261764.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Recog_2022826171650.mat</t>
+  </si>
+  <si>
+    <t>Eye2Use</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>AMC_PY21NO05</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO09</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO12</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO13</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO16</t>
+  </si>
+  <si>
+    <t>EDF</t>
+  </si>
+  <si>
+    <t>NO5171621.edf</t>
+  </si>
+  <si>
+    <t>NO5271621.edf</t>
+  </si>
+  <si>
+    <t>NO5171821.edf</t>
+  </si>
+  <si>
+    <t>NO5271821.edf</t>
+  </si>
+  <si>
+    <t>NO20221615110.edf</t>
+  </si>
+  <si>
+    <t>NO202216152152.edf</t>
+  </si>
+  <si>
+    <t>NO202217121946.edf</t>
+  </si>
+  <si>
+    <t>NO202217122836.edf</t>
+  </si>
+  <si>
+    <t>NO20221811515.edf</t>
+  </si>
+  <si>
+    <t>NO20221812052.edf</t>
+  </si>
+  <si>
+    <t>NO52022420124541.edf</t>
+  </si>
+  <si>
+    <t>NO52022420125453.edf</t>
+  </si>
+  <si>
+    <t>NO202252915450.edf</t>
+  </si>
+  <si>
+    <t>NO2022529151348.edf</t>
+  </si>
+  <si>
+    <t>NO202261115116.edf</t>
+  </si>
+  <si>
+    <t>NO20226111597.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105026.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105927.edf</t>
+  </si>
+  <si>
+    <t>NO2022826164318.edf</t>
+  </si>
+  <si>
+    <t>NO202282616539.edf</t>
+  </si>
+  <si>
+    <t>NO20228261764.edf</t>
+  </si>
+  <si>
+    <t>NO2022826171650.edf</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>Behavior</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221615110.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202216152152.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217121946.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217122836.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221811515.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221812052.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420124541.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420125453.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202252915450.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022529151348.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202261115116.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520226111597.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105026.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105927.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826164318.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202282616539.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520228261764.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826171650.txt</t>
+  </si>
+  <si>
+    <t>MatFile</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Learn_5171621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Recog_5271621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Learn_5171821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Recog_5271821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Learn_20221615110.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Recog_202216152152.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Learn_202217121946.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Recog_202217122836.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Learn_20221811515.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Recog_20221812052.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Learn_52022420124541.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Recog_52022420125453.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Learn_202252915450.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Recog_2022529151348.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Learn_202261115116.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Recog_20226111597.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Learn_2022527105026.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Recog_2022527105927.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Learn_2022826164318.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Recog_202282616539.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Learn_20228261764.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Recog_2022826171650.mat</t>
+  </si>
+  <si>
+    <t>Eye2Use</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>AMC_PY21NO05</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO09</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO12</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO13</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO16</t>
+  </si>
+  <si>
+    <t>EDF</t>
+  </si>
+  <si>
+    <t>NO5171621.edf</t>
+  </si>
+  <si>
+    <t>NO5271621.edf</t>
+  </si>
+  <si>
+    <t>NO5171821.edf</t>
+  </si>
+  <si>
+    <t>NO5271821.edf</t>
+  </si>
+  <si>
+    <t>NO20221615110.edf</t>
+  </si>
+  <si>
+    <t>NO202216152152.edf</t>
+  </si>
+  <si>
+    <t>NO202217121946.edf</t>
+  </si>
+  <si>
+    <t>NO202217122836.edf</t>
+  </si>
+  <si>
+    <t>NO20221811515.edf</t>
+  </si>
+  <si>
+    <t>NO20221812052.edf</t>
+  </si>
+  <si>
+    <t>NO52022420124541.edf</t>
+  </si>
+  <si>
+    <t>NO52022420125453.edf</t>
+  </si>
+  <si>
+    <t>NO202252915450.edf</t>
+  </si>
+  <si>
+    <t>NO2022529151348.edf</t>
+  </si>
+  <si>
+    <t>NO202261115116.edf</t>
+  </si>
+  <si>
+    <t>NO20226111597.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105026.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105927.edf</t>
+  </si>
+  <si>
+    <t>NO2022826164318.edf</t>
+  </si>
+  <si>
+    <t>NO202282616539.edf</t>
+  </si>
+  <si>
+    <t>NO20228261764.edf</t>
+  </si>
+  <si>
+    <t>NO2022826171650.edf</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>Behavior</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221615110.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202216152152.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217121946.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217122836.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221811515.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221812052.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420124541.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420125453.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202252915450.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022529151348.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202261115116.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520226111597.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105026.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105927.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826164318.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202282616539.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520228261764.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826171650.txt</t>
+  </si>
+  <si>
+    <t>MatFile</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Learn_5171621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Recog_5271621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Learn_5171821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Recog_5271821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Learn_20221615110.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Recog_202216152152.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Learn_202217121946.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Recog_202217122836.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Learn_20221811515.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Recog_20221812052.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Learn_52022420124541.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Recog_52022420125453.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Learn_202252915450.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Recog_2022529151348.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Learn_202261115116.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Recog_20226111597.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Learn_2022527105026.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Recog_2022527105927.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Learn_2022826164318.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Recog_202282616539.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Learn_20228261764.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Recog_2022826171650.mat</t>
+  </si>
+  <si>
+    <t>Eye2Use</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>AMC_PY21NO05</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO09</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO12</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO13</t>
+  </si>
+  <si>
+    <t>AMC_PY22NO16</t>
+  </si>
+  <si>
+    <t>EDF</t>
+  </si>
+  <si>
+    <t>NO5171621.edf</t>
+  </si>
+  <si>
+    <t>NO5271621.edf</t>
+  </si>
+  <si>
+    <t>NO5171821.edf</t>
+  </si>
+  <si>
+    <t>NO5271821.edf</t>
+  </si>
+  <si>
+    <t>NO20221615110.edf</t>
+  </si>
+  <si>
+    <t>NO202216152152.edf</t>
+  </si>
+  <si>
+    <t>NO202217121946.edf</t>
+  </si>
+  <si>
+    <t>NO202217122836.edf</t>
+  </si>
+  <si>
+    <t>NO20221811515.edf</t>
+  </si>
+  <si>
+    <t>NO20221812052.edf</t>
+  </si>
+  <si>
+    <t>NO52022420124541.edf</t>
+  </si>
+  <si>
+    <t>NO52022420125453.edf</t>
+  </si>
+  <si>
+    <t>NO202252915450.edf</t>
+  </si>
+  <si>
+    <t>NO2022529151348.edf</t>
+  </si>
+  <si>
+    <t>NO202261115116.edf</t>
+  </si>
+  <si>
+    <t>NO20226111597.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105026.edf</t>
+  </si>
+  <si>
+    <t>NO2022527105927.edf</t>
+  </si>
+  <si>
+    <t>NO2022826164318.edf</t>
+  </si>
+  <si>
+    <t>NO202282616539.edf</t>
+  </si>
+  <si>
+    <t>NO20228261764.edf</t>
+  </si>
+  <si>
+    <t>NO2022826171650.edf</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>learn</t>
+  </si>
+  <si>
+    <t>recog</t>
+  </si>
+  <si>
+    <t>Behavior</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.16.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Learning_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>MW5_Recognition_7.18.21.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221615110.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202216152152.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217121946.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202217122836.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221811515.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520221812052.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420124541.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022420125453.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202252915450.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022529151348.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202261115116.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520226111597.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105026.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022527105927.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826164318.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY5202282616539.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY520228261764.txt</t>
+  </si>
+  <si>
+    <t>NEWOLDDELAY52022826171650.txt</t>
+  </si>
+  <si>
+    <t>MatFile</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Learn_5171621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_1_Recog_5271621.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Learn_5171821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY21NO05_2_Recog_5271821.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Learn_20221615110.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_3_Recog_202216152152.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Learn_202217121946.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_1_Recog_202217122836.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Learn_20221811515.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO09_2_Recog_20221812052.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Learn_52022420124541.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO12_1_Recog_52022420125453.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Learn_202252915450.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_1_Recog_2022529151348.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Learn_202261115116.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_2_Recog_20226111597.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Learn_2022527105026.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO13_3_Recog_2022527105927.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Learn_2022826164318.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_1_Recog_202282616539.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Learn_20228261764.mat</t>
+  </si>
+  <si>
+    <t>eyetrack_AMC_PY22NO16_2_Recog_2022826171650.mat</t>
+  </si>
+  <si>
+    <t>Eye2Use</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
   </si>
   <si>
     <t>Subject</t>
@@ -1352,542 +2927,542 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="true"/>
-    <col min="2" max="2" width="21.046875" customWidth="true"/>
-    <col min="3" max="3" width="7.046875" customWidth="true"/>
-    <col min="4" max="4" width="5.7109375" customWidth="true"/>
-    <col min="5" max="5" width="30.7109375" customWidth="true"/>
-    <col min="6" max="6" width="49.48828125" customWidth="true"/>
-    <col min="7" max="7" width="8.15625" customWidth="true"/>
+    <col min="1" max="1" width="15.28515625" customWidth="true"/>
+    <col min="2" max="2" width="21.5703125" customWidth="true"/>
+    <col min="3" max="3" width="7.5703125" customWidth="true"/>
+    <col min="4" max="4" width="6" customWidth="true"/>
+    <col min="5" max="5" width="31.42578125" customWidth="true"/>
+    <col min="6" max="6" width="51.140625" customWidth="true"/>
+    <col min="7" max="7" width="8.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="0" t="s">
-        <v>211</v>
+        <v>736</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>217</v>
+        <v>742</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>240</v>
+        <v>765</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>241</v>
+        <v>766</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>264</v>
+        <v>789</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>287</v>
+        <v>812</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>310</v>
+        <v>835</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="0" t="s">
-        <v>212</v>
+        <v>737</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>218</v>
+        <v>743</v>
       </c>
       <c r="C2" s="0">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>242</v>
+        <v>767</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>265</v>
+        <v>790</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>288</v>
+        <v>813</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>311</v>
+        <v>836</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="0" t="s">
-        <v>212</v>
+        <v>737</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>219</v>
+        <v>744</v>
       </c>
       <c r="C3" s="0">
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>243</v>
+        <v>768</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>266</v>
+        <v>791</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>289</v>
+        <v>814</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>311</v>
+        <v>836</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="0" t="s">
-        <v>212</v>
+        <v>737</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>220</v>
+        <v>745</v>
       </c>
       <c r="C4" s="0">
         <v>2</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>244</v>
+        <v>769</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>267</v>
+        <v>792</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>290</v>
+        <v>815</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>311</v>
+        <v>836</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="0" t="s">
-        <v>212</v>
+        <v>737</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>221</v>
+        <v>746</v>
       </c>
       <c r="C5" s="0">
         <v>2</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>245</v>
+        <v>770</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>268</v>
+        <v>793</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>291</v>
+        <v>816</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>311</v>
+        <v>836</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="0" t="s">
-        <v>213</v>
+        <v>738</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>222</v>
+        <v>747</v>
       </c>
       <c r="C6" s="0">
         <v>3</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>246</v>
+        <v>771</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>269</v>
+        <v>794</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>292</v>
+        <v>817</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>312</v>
+        <v>837</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="0" t="s">
-        <v>213</v>
+        <v>738</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>223</v>
+        <v>748</v>
       </c>
       <c r="C7" s="0">
         <v>3</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>247</v>
+        <v>772</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>270</v>
+        <v>795</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>293</v>
+        <v>818</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>313</v>
+        <v>838</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="0" t="s">
-        <v>213</v>
+        <v>738</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>224</v>
+        <v>749</v>
       </c>
       <c r="C8" s="0">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>248</v>
+        <v>773</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>271</v>
+        <v>796</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>294</v>
+        <v>819</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>313</v>
+        <v>838</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="0" t="s">
-        <v>213</v>
+        <v>738</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>225</v>
+        <v>750</v>
       </c>
       <c r="C9" s="0">
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>249</v>
+        <v>774</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>272</v>
+        <v>797</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>295</v>
+        <v>820</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>313</v>
+        <v>838</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="0" t="s">
-        <v>213</v>
+        <v>738</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>226</v>
+        <v>751</v>
       </c>
       <c r="C10" s="0">
         <v>2</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>250</v>
+        <v>775</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>273</v>
+        <v>798</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>296</v>
+        <v>821</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="0" t="s">
-        <v>213</v>
+        <v>738</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>227</v>
+        <v>752</v>
       </c>
       <c r="C11" s="0">
         <v>2</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>251</v>
+        <v>776</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>274</v>
+        <v>799</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>297</v>
+        <v>822</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.25">
       <c r="A12" s="0" t="s">
-        <v>214</v>
+        <v>739</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>228</v>
+        <v>753</v>
       </c>
       <c r="C12" s="0">
         <v>3</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>252</v>
+        <v>777</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>275</v>
+        <v>800</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>298</v>
+        <v>823</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.25">
       <c r="A13" s="0" t="s">
-        <v>214</v>
+        <v>739</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>229</v>
+        <v>754</v>
       </c>
       <c r="C13" s="0">
         <v>3</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>253</v>
+        <v>778</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>276</v>
+        <v>801</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>299</v>
+        <v>824</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.25">
       <c r="A14" s="0" t="s">
-        <v>215</v>
+        <v>740</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>230</v>
+        <v>755</v>
       </c>
       <c r="C14" s="0">
         <v>1</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>254</v>
+        <v>779</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>277</v>
+        <v>802</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>300</v>
+        <v>825</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.25">
       <c r="A15" s="0" t="s">
-        <v>215</v>
+        <v>740</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>231</v>
+        <v>756</v>
       </c>
       <c r="C15" s="0">
         <v>1</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>255</v>
+        <v>780</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>278</v>
+        <v>803</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>301</v>
+        <v>826</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.25">
       <c r="A16" s="0" t="s">
-        <v>215</v>
+        <v>740</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>232</v>
+        <v>757</v>
       </c>
       <c r="C16" s="0">
         <v>2</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>256</v>
+        <v>781</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>279</v>
+        <v>804</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>302</v>
+        <v>827</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.25">
       <c r="A17" s="0" t="s">
-        <v>215</v>
+        <v>740</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>233</v>
+        <v>758</v>
       </c>
       <c r="C17" s="0">
         <v>2</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>257</v>
+        <v>782</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>280</v>
+        <v>805</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>303</v>
+        <v>828</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="18" x14ac:dyDescent="0.25">
       <c r="A18" s="0" t="s">
-        <v>215</v>
+        <v>740</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>234</v>
+        <v>759</v>
       </c>
       <c r="C18" s="0">
         <v>3</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>258</v>
+        <v>783</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>281</v>
+        <v>806</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>304</v>
+        <v>829</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.25">
       <c r="A19" s="0" t="s">
-        <v>215</v>
+        <v>740</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>235</v>
+        <v>760</v>
       </c>
       <c r="C19" s="0">
         <v>3</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>259</v>
+        <v>784</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>282</v>
+        <v>807</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>305</v>
+        <v>830</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.25">
       <c r="A20" s="0" t="s">
-        <v>216</v>
+        <v>741</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>236</v>
+        <v>761</v>
       </c>
       <c r="C20" s="0">
         <v>1</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>260</v>
+        <v>785</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>283</v>
+        <v>808</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>306</v>
+        <v>831</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.25">
       <c r="A21" s="0" t="s">
-        <v>216</v>
+        <v>741</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>237</v>
+        <v>762</v>
       </c>
       <c r="C21" s="0">
         <v>1</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>261</v>
+        <v>786</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>284</v>
+        <v>809</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>307</v>
+        <v>832</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="22" x14ac:dyDescent="0.25">
       <c r="A22" s="0" t="s">
-        <v>216</v>
+        <v>741</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>238</v>
+        <v>763</v>
       </c>
       <c r="C22" s="0">
         <v>2</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>262</v>
+        <v>787</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>285</v>
+        <v>810</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>308</v>
+        <v>833</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>314</v>
+        <v>839</v>
       </c>
     </row>
     <row r="23" x14ac:dyDescent="0.25">
       <c r="A23" s="0" t="s">
-        <v>216</v>
+        <v>741</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>239</v>
+        <v>764</v>
       </c>
       <c r="C23" s="0">
         <v>2</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>263</v>
+        <v>788</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>286</v>
+        <v>811</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>309</v>
+        <v>834</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>315</v>
+        <v>840</v>
       </c>
     </row>
   </sheetData>

</xml_diff>